<commit_message>
Prepared Expense Tracker for production (env + logging + error handling)
</commit_message>
<xml_diff>
--- a/expense-tracker/controllers/debug-report.xlsx
+++ b/expense-tracker/controllers/debug-report.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -36,31 +36,22 @@
     <t>Note</t>
   </si>
   <si>
-    <t>24/8/2025</t>
+    <t>29/8/2025</t>
   </si>
   <si>
     <t>Petrol</t>
   </si>
   <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t/>
+    <t>for car</t>
+  </si>
+  <si>
+    <t>salary</t>
   </si>
   <si>
     <t>Salary</t>
   </si>
   <si>
-    <t>25/8/2025</t>
-  </si>
-  <si>
-    <t>remember to eat</t>
-  </si>
-  <si>
-    <t>27/8/2025</t>
-  </si>
-  <si>
-    <t>For scooty</t>
+    <t>Yearly Salary</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -446,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -486,13 +477,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1000</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -500,81 +491,30 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1000000</v>
       </c>
       <c r="E5">
         <v>1000</v>
       </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6">
-        <v>1000</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8">
-        <v>200000</v>
-      </c>
-      <c r="E8">
-        <v>3000</v>
-      </c>
-      <c r="F8">
-        <v>197000</v>
+      <c r="F5">
+        <v>999000</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -608,30 +548,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>200000</v>
+        <v>1000000</v>
       </c>
       <c r="C2">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D2">
-        <v>197000</v>
+        <v>999000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>200000</v>
+        <v>1000000</v>
       </c>
       <c r="C4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <v>197000</v>
+        <v>999000</v>
       </c>
     </row>
   </sheetData>
@@ -659,18 +599,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>